<commit_message>
split the tibetic_grammars.R file into multiple .R files for each section.
</commit_message>
<xml_diff>
--- a/Tibetic-Grammars_Review_Master.xlsx
+++ b/Tibetic-Grammars_Review_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Projects\01_PhD\03_Analysis\02_TGR\tibetic_grammars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9F2697-D515-4F98-9FBA-19534D8245E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B5DFFC-77D8-4881-B28C-C378DF6EA2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24098" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{999B515B-97FA-46B5-AE4A-F4B530AC5BD1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{999B515B-97FA-46B5-AE4A-F4B530AC5BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="325">
   <si>
     <t>key</t>
   </si>
@@ -875,12 +875,6 @@
     <t>imp_pst_mentor</t>
   </si>
   <si>
-    <t>year_first_fw</t>
-  </si>
-  <si>
-    <t>total_time_fw</t>
-  </si>
-  <si>
     <t>data_source</t>
   </si>
   <si>
@@ -914,9 +908,6 @@
     <t>data_where</t>
   </si>
   <si>
-    <t>ierb_ethics_mention</t>
-  </si>
-  <si>
     <t>consent_mention</t>
   </si>
   <si>
@@ -965,9 +956,6 @@
     <t>example_source</t>
   </si>
   <si>
-    <t>_</t>
-  </si>
-  <si>
     <t>An Introduction to the Grammar of the Tibetan Language with the texts of Situ sum_tag, Dag_je salwai me_long, and Situi shal lung</t>
   </si>
   <si>
@@ -1008,6 +996,21 @@
   </si>
   <si>
     <t>Merak_Sakteng</t>
+  </si>
+  <si>
+    <t>irb_ethics_info</t>
+  </si>
+  <si>
+    <t>year_first_ft</t>
+  </si>
+  <si>
+    <t>85 [104]</t>
+  </si>
+  <si>
+    <t>OF+PS+US</t>
+  </si>
+  <si>
+    <t>total_years_grammar</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1064,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1081,6 +1084,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1418,8 +1422,8 @@
   <dimension ref="A1:BO31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF25" sqref="AF25"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1500,55 +1504,55 @@
         <v>11</v>
       </c>
       <c r="W1" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="Y1" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>290</v>
       </c>
       <c r="AI1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="AJ1" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="AM1" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>294</v>
       </c>
       <c r="AN1" s="3" t="s">
         <v>13</v>
@@ -1557,22 +1561,22 @@
         <v>14</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="AS1" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>300</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>15</v>
@@ -1596,7 +1600,7 @@
         <v>21</v>
       </c>
       <c r="BC1" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="BD1" s="3" t="s">
         <v>22</v>
@@ -1611,28 +1615,28 @@
         <v>25</v>
       </c>
       <c r="BH1" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="BK1" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="BJ1" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="BK1" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="BL1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="BM1" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="BN1" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="BO1" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.45">
@@ -1708,7 +1712,7 @@
       <c r="X2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>208</v>
       </c>
       <c r="Z2" s="3" t="s">
@@ -1854,8 +1858,8 @@
       <c r="E3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>309</v>
+      <c r="F3" s="7" t="s">
+        <v>322</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -1911,7 +1915,7 @@
       <c r="X3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Y3" s="2" t="s">
         <v>208</v>
       </c>
       <c r="Z3" s="3" t="s">
@@ -2114,7 +2118,7 @@
       <c r="X4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" s="2" t="s">
         <v>208</v>
       </c>
       <c r="Z4" s="3" t="s">
@@ -2258,7 +2262,7 @@
         <v>121</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>57</v>
@@ -2317,7 +2321,7 @@
       <c r="X5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="Y5" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Z5" s="3" t="s">
@@ -2520,7 +2524,7 @@
       <c r="X6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y6" s="3" t="s">
+      <c r="Y6" s="2" t="s">
         <v>69</v>
       </c>
       <c r="Z6" s="3" t="s">
@@ -2723,7 +2727,7 @@
       <c r="X7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y7" s="3" t="s">
+      <c r="Y7" s="1" t="s">
         <v>77</v>
       </c>
       <c r="Z7" s="3" t="s">
@@ -2926,7 +2930,7 @@
       <c r="X8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y8" s="3" t="s">
+      <c r="Y8" s="2" t="s">
         <v>208</v>
       </c>
       <c r="Z8" s="3" t="s">
@@ -3106,7 +3110,7 @@
         <v>35</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>34</v>
@@ -3129,7 +3133,7 @@
       <c r="X9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y9" s="3" t="s">
+      <c r="Y9" s="2" t="s">
         <v>208</v>
       </c>
       <c r="Z9" s="3" t="s">
@@ -3332,7 +3336,7 @@
       <c r="X10" s="3">
         <v>8</v>
       </c>
-      <c r="Y10" s="3" t="s">
+      <c r="Y10" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z10" s="3" t="s">
@@ -3384,7 +3388,7 @@
         <v>54</v>
       </c>
       <c r="AP10" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AQ10" s="3" t="s">
         <v>32</v>
@@ -3535,7 +3539,7 @@
       <c r="X11" s="3">
         <v>9</v>
       </c>
-      <c r="Y11" s="3" t="s">
+      <c r="Y11" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z11" s="3" t="s">
@@ -3738,7 +3742,7 @@
       <c r="X12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y12" s="3" t="s">
+      <c r="Y12" s="1" t="s">
         <v>208</v>
       </c>
       <c r="Z12" s="3" t="s">
@@ -3938,7 +3942,7 @@
       <c r="X13" s="3">
         <v>4</v>
       </c>
-      <c r="Y13" s="3" t="s">
+      <c r="Y13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="Z13" s="3" t="s">
@@ -4141,7 +4145,7 @@
       <c r="X14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y14" s="3" t="s">
+      <c r="Y14" s="2" t="s">
         <v>208</v>
       </c>
       <c r="Z14" s="3" t="s">
@@ -4309,7 +4313,7 @@
         <v>51</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>32</v>
@@ -4321,7 +4325,7 @@
         <v>35</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="R15" s="3" t="s">
         <v>34</v>
@@ -4344,7 +4348,7 @@
       <c r="X15" s="3">
         <v>6</v>
       </c>
-      <c r="Y15" s="3" t="s">
+      <c r="Y15" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z15" s="3" t="s">
@@ -4497,7 +4501,7 @@
         <v>10</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>129</v>
@@ -4547,7 +4551,7 @@
       <c r="X16" s="3">
         <v>7</v>
       </c>
-      <c r="Y16" s="3" t="s">
+      <c r="Y16" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z16" s="3" t="s">
@@ -4750,7 +4754,7 @@
       <c r="X17" s="3">
         <v>4</v>
       </c>
-      <c r="Y17" s="3" t="s">
+      <c r="Y17" s="2" t="s">
         <v>100</v>
       </c>
       <c r="Z17" s="3" t="s">
@@ -4953,7 +4957,7 @@
       <c r="X18" s="3">
         <v>5</v>
       </c>
-      <c r="Y18" s="3" t="s">
+      <c r="Y18" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z18" s="3" t="s">
@@ -5156,7 +5160,7 @@
       <c r="X19" s="3">
         <v>14</v>
       </c>
-      <c r="Y19" s="3" t="s">
+      <c r="Y19" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z19" s="3" t="s">
@@ -5324,7 +5328,7 @@
         <v>51</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>32</v>
@@ -5359,7 +5363,7 @@
       <c r="X20" s="3">
         <v>30</v>
       </c>
-      <c r="Y20" s="3" t="s">
+      <c r="Y20" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z20" s="3" t="s">
@@ -5411,7 +5415,7 @@
         <v>54</v>
       </c>
       <c r="AP20" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AQ20" s="3" t="s">
         <v>32</v>
@@ -5562,7 +5566,7 @@
       <c r="X21" s="3">
         <v>9</v>
       </c>
-      <c r="Y21" s="3" t="s">
+      <c r="Y21" s="2" t="s">
         <v>100</v>
       </c>
       <c r="Z21" s="3" t="s">
@@ -5765,7 +5769,7 @@
       <c r="X22" s="3">
         <v>44</v>
       </c>
-      <c r="Y22" s="3" t="s">
+      <c r="Y22" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z22" s="3" t="s">
@@ -5918,7 +5922,7 @@
         <v>8</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>129</v>
@@ -5968,7 +5972,7 @@
       <c r="X23" s="3">
         <v>7</v>
       </c>
-      <c r="Y23" s="3" t="s">
+      <c r="Y23" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z23" s="3" t="s">
@@ -6171,7 +6175,7 @@
       <c r="X24" s="3">
         <v>14</v>
       </c>
-      <c r="Y24" s="3" t="s">
+      <c r="Y24" s="2" t="s">
         <v>100</v>
       </c>
       <c r="Z24" s="3" t="s">
@@ -6374,8 +6378,8 @@
       <c r="X25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y25" s="3" t="s">
-        <v>100</v>
+      <c r="Y25" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="Z25" s="3" t="s">
         <v>39</v>
@@ -6396,7 +6400,7 @@
         <v>39</v>
       </c>
       <c r="AF25" s="1" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="AG25" s="3" t="s">
         <v>35</v>
@@ -6426,7 +6430,7 @@
         <v>203</v>
       </c>
       <c r="AP25" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="AQ25" s="3" t="s">
         <v>39</v>
@@ -6577,8 +6581,8 @@
       <c r="X26" s="3">
         <v>15</v>
       </c>
-      <c r="Y26" s="3" t="s">
-        <v>100</v>
+      <c r="Y26" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="Z26" s="3" t="s">
         <v>39</v>
@@ -6629,7 +6633,7 @@
         <v>203</v>
       </c>
       <c r="AP26" s="3" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="AQ26" s="3" t="s">
         <v>32</v>
@@ -6780,7 +6784,7 @@
       <c r="X27" s="3">
         <v>9</v>
       </c>
-      <c r="Y27" s="3" t="s">
+      <c r="Y27" s="2" t="s">
         <v>77</v>
       </c>
       <c r="Z27" s="3" t="s">
@@ -6832,7 +6836,7 @@
         <v>54</v>
       </c>
       <c r="AP27" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AQ27" s="3" t="s">
         <v>32</v>
@@ -6983,7 +6987,7 @@
       <c r="X28" s="3">
         <v>3</v>
       </c>
-      <c r="Y28" s="3" t="s">
+      <c r="Y28" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z28" s="3" t="s">
@@ -7127,7 +7131,7 @@
         <v>44</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>244</v>
@@ -7151,7 +7155,7 @@
         <v>51</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="N29" s="6" t="s">
         <v>39</v>
@@ -7183,7 +7187,7 @@
       <c r="X29" s="3">
         <v>17</v>
       </c>
-      <c r="Y29" s="3" t="s">
+      <c r="Y29" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z29" s="3" t="s">
@@ -7386,7 +7390,7 @@
       <c r="X30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Y30" s="3" t="s">
+      <c r="Y30" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z30" s="3" t="s">
@@ -7589,7 +7593,7 @@
       <c r="X31" s="3">
         <v>13</v>
       </c>
-      <c r="Y31" s="3" t="s">
+      <c r="Y31" s="1" t="s">
         <v>100</v>
       </c>
       <c r="Z31" s="3" t="s">

</xml_diff>

<commit_message>
Added example source plots and various other plots in the tg_examples.R file
</commit_message>
<xml_diff>
--- a/Tibetic-Grammars_Review_Master.xlsx
+++ b/Tibetic-Grammars_Review_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Projects\01_PhD\03_Analysis\02_TGR\tibetic_grammars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B5DFFC-77D8-4881-B28C-C378DF6EA2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D44465-931B-4E93-B724-DD7AFB009E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{999B515B-97FA-46B5-AE4A-F4B530AC5BD1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="324">
   <si>
     <t>key</t>
   </si>
@@ -404,9 +404,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>E+NS+PS</t>
-  </si>
-  <si>
     <t>DenwoodP1999</t>
   </si>
   <si>
@@ -689,9 +686,6 @@
     <t>Some by IU, mostly by whole sentences</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>YliniemiJ2019</t>
   </si>
   <si>
@@ -938,18 +932,12 @@
     <t>multi_modal_anal</t>
   </si>
   <si>
-    <t>exmaple_IG</t>
-  </si>
-  <si>
     <t>n_tiers</t>
   </si>
   <si>
     <t>nat_orth</t>
   </si>
   <si>
-    <t>abbreviation_list</t>
-  </si>
-  <si>
     <t>example_citation_LS</t>
   </si>
   <si>
@@ -1011,6 +999,15 @@
   </si>
   <si>
     <t>total_years_grammar</t>
+  </si>
+  <si>
+    <t>example_ig</t>
+  </si>
+  <si>
+    <t>abbreviations</t>
+  </si>
+  <si>
+    <t>E+NS+OS</t>
   </si>
 </sst>
 </file>
@@ -1421,9 +1418,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B25BD2-0404-4F41-955D-7B511D9709C2}">
   <dimension ref="A1:BO31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AW1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BH24" sqref="BH24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1447,22 +1444,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>5</v>
@@ -1474,7 +1471,7 @@
         <v>7</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>8</v>
@@ -1483,76 +1480,76 @@
         <v>9</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>276</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="Y1" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA1" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>286</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>288</v>
       </c>
       <c r="AI1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="AJ1" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="AM1" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>291</v>
       </c>
       <c r="AN1" s="3" t="s">
         <v>13</v>
@@ -1561,22 +1558,22 @@
         <v>14</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="AR1" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="AV1" s="3" t="s">
         <v>15</v>
@@ -1600,7 +1597,7 @@
         <v>21</v>
       </c>
       <c r="BC1" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="BD1" s="3" t="s">
         <v>22</v>
@@ -1615,28 +1612,28 @@
         <v>25</v>
       </c>
       <c r="BH1" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="BK1" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="BJ1" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="BK1" s="3" t="s">
-        <v>302</v>
       </c>
       <c r="BL1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="BM1" s="3" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="BN1" s="3" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="BO1" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.45">
@@ -1713,7 +1710,7 @@
         <v>35</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>34</v>
@@ -1838,7 +1835,7 @@
       <c r="BN2" s="5">
         <v>1</v>
       </c>
-      <c r="BO2" s="3" t="s">
+      <c r="BO2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1859,7 +1856,7 @@
         <v>42</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -1916,7 +1913,7 @@
         <v>35</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z3" s="3" t="s">
         <v>34</v>
@@ -2041,7 +2038,7 @@
       <c r="BN3" s="5">
         <v>1</v>
       </c>
-      <c r="BO3" s="3" t="s">
+      <c r="BO3" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2119,7 +2116,7 @@
         <v>35</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z4" s="3" t="s">
         <v>34</v>
@@ -2244,7 +2241,7 @@
       <c r="BN4" s="5">
         <v>1</v>
       </c>
-      <c r="BO4" s="3" t="s">
+      <c r="BO4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2262,7 +2259,7 @@
         <v>121</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>57</v>
@@ -2447,7 +2444,7 @@
       <c r="BN5" s="5">
         <v>1</v>
       </c>
-      <c r="BO5" s="3" t="s">
+      <c r="BO5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2650,7 +2647,7 @@
       <c r="BN6" s="5">
         <v>1</v>
       </c>
-      <c r="BO6" s="3" t="s">
+      <c r="BO6" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2686,7 +2683,7 @@
         <v>75</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>51</v>
@@ -2853,7 +2850,7 @@
       <c r="BN7" s="6">
         <v>1</v>
       </c>
-      <c r="BO7" s="3" t="s">
+      <c r="BO7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2889,7 +2886,7 @@
         <v>83</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>34</v>
@@ -2931,7 +2928,7 @@
         <v>35</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>34</v>
@@ -3056,7 +3053,7 @@
       <c r="BN8" s="5">
         <v>1</v>
       </c>
-      <c r="BO8" s="3" t="s">
+      <c r="BO8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3110,7 +3107,7 @@
         <v>35</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>34</v>
@@ -3134,7 +3131,7 @@
         <v>35</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z9" s="3" t="s">
         <v>34</v>
@@ -3259,7 +3256,7 @@
       <c r="BN9" s="5">
         <v>1</v>
       </c>
-      <c r="BO9" s="3" t="s">
+      <c r="BO9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3295,7 +3292,7 @@
         <v>97</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>44</v>
@@ -3388,7 +3385,7 @@
         <v>54</v>
       </c>
       <c r="AP10" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="AQ10" s="3" t="s">
         <v>32</v>
@@ -3462,7 +3459,7 @@
       <c r="BN10" s="6">
         <v>1</v>
       </c>
-      <c r="BO10" s="3" t="s">
+      <c r="BO10" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3498,7 +3495,7 @@
         <v>105</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>34</v>
@@ -3665,7 +3662,7 @@
       <c r="BN11" s="6">
         <v>1</v>
       </c>
-      <c r="BO11" s="3" t="s">
+      <c r="BO11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3743,7 +3740,7 @@
         <v>35</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>70</v>
@@ -3868,7 +3865,7 @@
       <c r="BN12" s="6">
         <v>1</v>
       </c>
-      <c r="BO12" s="3" t="s">
+      <c r="BO12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3904,7 +3901,7 @@
         <v>117</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>34</v>
@@ -4068,16 +4065,16 @@
       <c r="BN13" s="6">
         <v>2</v>
       </c>
-      <c r="BO13" s="3" t="s">
-        <v>122</v>
+      <c r="BO13" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="C14" s="3">
         <v>1999</v>
@@ -4089,13 +4086,13 @@
         <v>33</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G14" s="3">
         <v>15</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>32</v>
@@ -4122,7 +4119,7 @@
         <v>35</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>34</v>
@@ -4146,7 +4143,7 @@
         <v>35</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z14" s="3" t="s">
         <v>34</v>
@@ -4197,7 +4194,7 @@
         <v>54</v>
       </c>
       <c r="AP14" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AQ14" s="3" t="s">
         <v>32</v>
@@ -4260,7 +4257,7 @@
         <v>4</v>
       </c>
       <c r="BK14" s="3" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="BL14" s="3" t="s">
         <v>35</v>
@@ -4271,16 +4268,16 @@
       <c r="BN14" s="5">
         <v>1</v>
       </c>
-      <c r="BO14" s="3" t="s">
+      <c r="BO14" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="C15" s="3">
         <v>2004</v>
@@ -4289,31 +4286,31 @@
         <v>44</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="G15" s="3">
         <v>5</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="K15" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>51</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>32</v>
@@ -4325,7 +4322,7 @@
         <v>35</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="R15" s="3" t="s">
         <v>34</v>
@@ -4474,16 +4471,16 @@
       <c r="BN15" s="6">
         <v>1</v>
       </c>
-      <c r="BO15" s="3" t="s">
-        <v>136</v>
+      <c r="BO15" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="C16" s="3">
         <v>2005</v>
@@ -4492,22 +4489,22 @@
         <v>44</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="G16" s="3">
         <v>10</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>91</v>
@@ -4516,7 +4513,7 @@
         <v>51</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>39</v>
@@ -4537,10 +4534,10 @@
         <v>34</v>
       </c>
       <c r="T16" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="U16" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="U16" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="V16" s="3" t="s">
         <v>32</v>
@@ -4677,16 +4674,16 @@
       <c r="BN16" s="6">
         <v>1</v>
       </c>
-      <c r="BO16" s="3" t="s">
+      <c r="BO16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="C17" s="3">
         <v>2007</v>
@@ -4695,10 +4692,10 @@
         <v>44</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="G17" s="3">
         <v>7</v>
@@ -4710,37 +4707,37 @@
         <v>39</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L17" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="N17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="N17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O17" s="3" t="s">
+      <c r="P17" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T17" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T17" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="U17" s="3" t="s">
         <v>34</v>
@@ -4806,7 +4803,7 @@
         <v>54</v>
       </c>
       <c r="AP17" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AQ17" s="3" t="s">
         <v>32</v>
@@ -4880,16 +4877,16 @@
       <c r="BN17" s="5">
         <v>1</v>
       </c>
-      <c r="BO17" s="3" t="s">
+      <c r="BO17" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="C18" s="3">
         <v>2007</v>
@@ -4898,10 +4895,10 @@
         <v>44</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="G18" s="3">
         <v>12</v>
@@ -4913,37 +4910,37 @@
         <v>39</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>51</v>
       </c>
       <c r="M18" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="N18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O18" s="3" t="s">
+      <c r="P18" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S18" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="P18" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S18" s="3" t="s">
+      <c r="T18" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="T18" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="U18" s="3" t="s">
         <v>34</v>
@@ -5083,16 +5080,16 @@
       <c r="BN18" s="6">
         <v>4</v>
       </c>
-      <c r="BO18" s="3" t="s">
-        <v>136</v>
+      <c r="BO18" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="C19" s="3">
         <v>2009</v>
@@ -5101,22 +5098,22 @@
         <v>44</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="G19" s="3">
         <v>7</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>38</v>
@@ -5137,7 +5134,7 @@
         <v>35</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>34</v>
@@ -5286,16 +5283,16 @@
       <c r="BN19" s="6">
         <v>1</v>
       </c>
-      <c r="BO19" s="3" t="s">
+      <c r="BO19" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="C20" s="3">
         <v>2010</v>
@@ -5304,31 +5301,31 @@
         <v>44</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="G20" s="3">
         <v>8</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="K20" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>51</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>32</v>
@@ -5340,19 +5337,19 @@
         <v>35</v>
       </c>
       <c r="Q20" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U20" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U20" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="V20" s="3" t="s">
         <v>32</v>
@@ -5415,7 +5412,7 @@
         <v>54</v>
       </c>
       <c r="AP20" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="AQ20" s="3" t="s">
         <v>32</v>
@@ -5489,16 +5486,16 @@
       <c r="BN20" s="6">
         <v>1</v>
       </c>
-      <c r="BO20" s="3" t="s">
+      <c r="BO20" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="C21" s="3">
         <v>2013</v>
@@ -5507,10 +5504,10 @@
         <v>44</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="G21" s="3">
         <v>8</v>
@@ -5525,13 +5522,13 @@
         <v>105</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>51</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>32</v>
@@ -5555,7 +5552,7 @@
         <v>107</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V21" s="3" t="s">
         <v>32</v>
@@ -5618,7 +5615,7 @@
         <v>54</v>
       </c>
       <c r="AP21" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AQ21" s="3" t="s">
         <v>32</v>
@@ -5692,16 +5689,16 @@
       <c r="BN21" s="5">
         <v>1</v>
       </c>
-      <c r="BO21" s="3" t="s">
+      <c r="BO21" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>187</v>
       </c>
       <c r="C22" s="3">
         <v>2016</v>
@@ -5710,31 +5707,31 @@
         <v>44</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>189</v>
       </c>
       <c r="G22" s="3">
         <v>19</v>
       </c>
       <c r="H22" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="K22" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L22" s="3" t="s">
         <v>51</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>39</v>
@@ -5746,7 +5743,7 @@
         <v>35</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>34</v>
@@ -5895,16 +5892,16 @@
       <c r="BN22" s="6">
         <v>2</v>
       </c>
-      <c r="BO22" s="3" t="s">
-        <v>136</v>
+      <c r="BO22" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="C23" s="3">
         <v>2016</v>
@@ -5913,44 +5910,44 @@
         <v>44</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="G23" s="3">
         <v>8</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>51</v>
       </c>
       <c r="M23" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q23" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="N23" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="R23" s="3" t="s">
         <v>34</v>
       </c>
@@ -5958,7 +5955,7 @@
         <v>34</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U23" s="3" t="s">
         <v>34</v>
@@ -5979,7 +5976,7 @@
         <v>39</v>
       </c>
       <c r="AA23" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AB23" s="6" t="s">
         <v>39</v>
@@ -6003,10 +6000,10 @@
         <v>39</v>
       </c>
       <c r="AI23" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ23" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="AJ23" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="AK23" s="3" t="s">
         <v>32</v>
@@ -6021,7 +6018,7 @@
         <v>37</v>
       </c>
       <c r="AO23" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AP23" s="3" t="s">
         <v>34</v>
@@ -6098,16 +6095,16 @@
       <c r="BN23" s="6">
         <v>4</v>
       </c>
-      <c r="BO23" s="3" t="s">
-        <v>122</v>
+      <c r="BO23" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C24" s="3">
         <v>2018</v>
@@ -6116,31 +6113,31 @@
         <v>44</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="G24" s="3">
         <v>7</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>105</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>51</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N24" s="6" t="s">
         <v>32</v>
@@ -6164,7 +6161,7 @@
         <v>107</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="V24" s="3" t="s">
         <v>32</v>
@@ -6301,16 +6298,16 @@
       <c r="BN24" s="5">
         <v>1</v>
       </c>
-      <c r="BO24" s="3" t="s">
-        <v>208</v>
+      <c r="BO24" s="2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="C25" s="3">
         <v>2018</v>
@@ -6319,10 +6316,10 @@
         <v>44</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="G25" s="3">
         <v>12</v>
@@ -6349,25 +6346,25 @@
         <v>32</v>
       </c>
       <c r="O25" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="T25" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="P25" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S25" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="T25" s="3" t="s">
+      <c r="U25" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="U25" s="3" t="s">
-        <v>215</v>
       </c>
       <c r="V25" s="3" t="s">
         <v>32</v>
@@ -6427,16 +6424,16 @@
         <v>37</v>
       </c>
       <c r="AO25" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AP25" s="3" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="AQ25" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AR25" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AS25" s="3" t="s">
         <v>121</v>
@@ -6493,7 +6490,7 @@
         <v>3</v>
       </c>
       <c r="BK25" s="3" t="s">
-        <v>217</v>
+        <v>39</v>
       </c>
       <c r="BL25" s="3" t="s">
         <v>32</v>
@@ -6504,16 +6501,16 @@
       <c r="BN25" s="6">
         <v>3</v>
       </c>
-      <c r="BO25" s="3" t="s">
-        <v>136</v>
+      <c r="BO25" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C26" s="3">
         <v>2019</v>
@@ -6522,10 +6519,10 @@
         <v>44</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G26" s="3">
         <v>17</v>
@@ -6537,7 +6534,7 @@
         <v>39</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>38</v>
@@ -6546,13 +6543,13 @@
         <v>44</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N26" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P26" s="3" t="s">
         <v>119</v>
@@ -6564,13 +6561,13 @@
         <v>34</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="U26" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="V26" s="3" t="s">
         <v>32</v>
@@ -6582,13 +6579,13 @@
         <v>15</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="Z26" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AA26" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AB26" s="6" t="s">
         <v>39</v>
@@ -6615,7 +6612,7 @@
         <v>35</v>
       </c>
       <c r="AJ26" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK26" s="3" t="s">
         <v>39</v>
@@ -6630,10 +6627,10 @@
         <v>37</v>
       </c>
       <c r="AO26" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AP26" s="3" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AQ26" s="3" t="s">
         <v>32</v>
@@ -6707,16 +6704,16 @@
       <c r="BN26" s="6">
         <v>4</v>
       </c>
-      <c r="BO26" s="3" t="s">
-        <v>136</v>
+      <c r="BO26" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C27" s="3">
         <v>2019</v>
@@ -6725,10 +6722,10 @@
         <v>44</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G27" s="3">
         <v>11</v>
@@ -6740,10 +6737,10 @@
         <v>39</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>44</v>
@@ -6755,22 +6752,22 @@
         <v>32</v>
       </c>
       <c r="O27" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="S27" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T27" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q27" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R27" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="S27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T27" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="U27" s="3" t="s">
         <v>34</v>
@@ -6836,7 +6833,7 @@
         <v>54</v>
       </c>
       <c r="AP27" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AQ27" s="3" t="s">
         <v>32</v>
@@ -6910,16 +6907,16 @@
       <c r="BN27" s="5">
         <v>2</v>
       </c>
-      <c r="BO27" s="3" t="s">
-        <v>122</v>
+      <c r="BO27" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C28" s="3">
         <v>2020</v>
@@ -6928,22 +6925,22 @@
         <v>44</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G28" s="3">
         <v>9</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>32</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>38</v>
@@ -6952,7 +6949,7 @@
         <v>51</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N28" s="6" t="s">
         <v>39</v>
@@ -7113,16 +7110,16 @@
       <c r="BN28" s="6">
         <v>2</v>
       </c>
-      <c r="BO28" s="3" t="s">
-        <v>136</v>
+      <c r="BO28" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C29" s="3">
         <v>2021</v>
@@ -7131,10 +7128,10 @@
         <v>44</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G29" s="3">
         <v>16</v>
@@ -7146,7 +7143,7 @@
         <v>39</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>38</v>
@@ -7155,28 +7152,28 @@
         <v>51</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="N29" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O29" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T29" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="V29" s="3" t="s">
         <v>32</v>
@@ -7239,7 +7236,7 @@
         <v>54</v>
       </c>
       <c r="AP29" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AQ29" s="3" t="s">
         <v>32</v>
@@ -7313,16 +7310,16 @@
       <c r="BN29" s="6">
         <v>1</v>
       </c>
-      <c r="BO29" s="3" t="s">
+      <c r="BO29" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C30" s="3">
         <v>2021</v>
@@ -7331,10 +7328,10 @@
         <v>44</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G30" s="3">
         <v>6</v>
@@ -7346,7 +7343,7 @@
         <v>39</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>38</v>
@@ -7355,28 +7352,28 @@
         <v>51</v>
       </c>
       <c r="M30" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="P30" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="N30" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="O30" s="3" t="s">
+      <c r="Q30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T30" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="P30" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="R30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="S30" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T30" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="U30" s="3" t="s">
         <v>34</v>
@@ -7516,16 +7513,16 @@
       <c r="BN30" s="6">
         <v>1</v>
       </c>
-      <c r="BO30" s="3" t="s">
+      <c r="BO30" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:67" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C31" s="3">
         <v>2022</v>
@@ -7534,43 +7531,43 @@
         <v>44</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G31" s="3">
         <v>5</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>32</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L31" s="3" t="s">
         <v>51</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="N31" s="6" t="s">
         <v>39</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="P31" s="3" t="s">
         <v>119</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="R31" s="3" t="s">
         <v>34</v>
@@ -7719,7 +7716,7 @@
       <c r="BN31" s="6">
         <v>1</v>
       </c>
-      <c r="BO31" s="3" t="s">
+      <c r="BO31" s="1" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added plots to coverage and added more plots to examples and backmatter.
</commit_message>
<xml_diff>
--- a/Tibetic-Grammars_Review_Master.xlsx
+++ b/Tibetic-Grammars_Review_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_Projects\01_PhD\03_Analysis\02_TGR\tibetic_grammars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D44465-931B-4E93-B724-DD7AFB009E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66DDA78-14CA-4409-B1E3-1C7B817593D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{999B515B-97FA-46B5-AE4A-F4B530AC5BD1}"/>
   </bookViews>
@@ -1418,9 +1418,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B25BD2-0404-4F41-955D-7B511D9709C2}">
   <dimension ref="A1:BO31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BH24" sqref="BH24"/>
+      <selection pane="topRight" activeCell="AY11" sqref="AY11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1832,7 +1832,7 @@
       <c r="BM2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BN2" s="5">
+      <c r="BN2" s="2">
         <v>1</v>
       </c>
       <c r="BO2" s="1" t="s">
@@ -2035,7 +2035,7 @@
       <c r="BM3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN3" s="5">
+      <c r="BN3" s="2">
         <v>1</v>
       </c>
       <c r="BO3" s="2" t="s">
@@ -2238,7 +2238,7 @@
       <c r="BM4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BN4" s="5">
+      <c r="BN4" s="2">
         <v>1</v>
       </c>
       <c r="BO4" s="1" t="s">
@@ -2441,7 +2441,7 @@
       <c r="BM5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN5" s="5">
+      <c r="BN5" s="2">
         <v>1</v>
       </c>
       <c r="BO5" s="1" t="s">
@@ -2644,7 +2644,7 @@
       <c r="BM6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN6" s="5">
+      <c r="BN6" s="2">
         <v>1</v>
       </c>
       <c r="BO6" s="1" t="s">
@@ -2847,7 +2847,7 @@
       <c r="BM7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BN7" s="6">
+      <c r="BN7" s="1">
         <v>1</v>
       </c>
       <c r="BO7" s="1" t="s">
@@ -3050,7 +3050,7 @@
       <c r="BM8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN8" s="5">
+      <c r="BN8" s="2">
         <v>1</v>
       </c>
       <c r="BO8" s="2" t="s">
@@ -3253,7 +3253,7 @@
       <c r="BM9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN9" s="5">
+      <c r="BN9" s="2">
         <v>1</v>
       </c>
       <c r="BO9" s="1" t="s">
@@ -3456,7 +3456,7 @@
       <c r="BM10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN10" s="6">
+      <c r="BN10" s="1">
         <v>1</v>
       </c>
       <c r="BO10" s="1" t="s">
@@ -3659,7 +3659,7 @@
       <c r="BM11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN11" s="6">
+      <c r="BN11" s="1">
         <v>1</v>
       </c>
       <c r="BO11" s="1" t="s">
@@ -3862,7 +3862,7 @@
       <c r="BM12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN12" s="6">
+      <c r="BN12" s="1">
         <v>1</v>
       </c>
       <c r="BO12" s="1" t="s">
@@ -4062,7 +4062,7 @@
       <c r="BM13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN13" s="6">
+      <c r="BN13" s="1">
         <v>2</v>
       </c>
       <c r="BO13" s="1" t="s">
@@ -4265,7 +4265,7 @@
       <c r="BM14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN14" s="5">
+      <c r="BN14" s="2">
         <v>1</v>
       </c>
       <c r="BO14" s="2" t="s">
@@ -4468,7 +4468,7 @@
       <c r="BM15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN15" s="6">
+      <c r="BN15" s="1">
         <v>1</v>
       </c>
       <c r="BO15" s="1" t="s">
@@ -4671,7 +4671,7 @@
       <c r="BM16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN16" s="6">
+      <c r="BN16" s="1">
         <v>1</v>
       </c>
       <c r="BO16" s="1" t="s">
@@ -4874,7 +4874,7 @@
       <c r="BM17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN17" s="5">
+      <c r="BN17" s="2">
         <v>1</v>
       </c>
       <c r="BO17" s="2" t="s">
@@ -5077,7 +5077,7 @@
       <c r="BM18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN18" s="6">
+      <c r="BN18" s="1">
         <v>4</v>
       </c>
       <c r="BO18" s="1" t="s">
@@ -5280,7 +5280,7 @@
       <c r="BM19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="BN19" s="6">
+      <c r="BN19" s="1">
         <v>1</v>
       </c>
       <c r="BO19" s="1" t="s">
@@ -5483,7 +5483,7 @@
       <c r="BM20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN20" s="6">
+      <c r="BN20" s="1">
         <v>1</v>
       </c>
       <c r="BO20" s="1" t="s">
@@ -5686,7 +5686,7 @@
       <c r="BM21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN21" s="5">
+      <c r="BN21" s="2">
         <v>1</v>
       </c>
       <c r="BO21" s="2" t="s">
@@ -5889,7 +5889,7 @@
       <c r="BM22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN22" s="6">
+      <c r="BN22" s="1">
         <v>2</v>
       </c>
       <c r="BO22" s="1" t="s">
@@ -6092,8 +6092,8 @@
       <c r="BM23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN23" s="6">
-        <v>4</v>
+      <c r="BN23" s="1">
+        <v>5</v>
       </c>
       <c r="BO23" s="1" t="s">
         <v>323</v>
@@ -6295,7 +6295,7 @@
       <c r="BM24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN24" s="5">
+      <c r="BN24" s="2">
         <v>1</v>
       </c>
       <c r="BO24" s="2" t="s">
@@ -6498,7 +6498,7 @@
       <c r="BM25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN25" s="6">
+      <c r="BN25" s="1">
         <v>3</v>
       </c>
       <c r="BO25" s="1" t="s">
@@ -6701,8 +6701,8 @@
       <c r="BM26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN26" s="6">
-        <v>4</v>
+      <c r="BN26" s="1">
+        <v>3</v>
       </c>
       <c r="BO26" s="1" t="s">
         <v>323</v>
@@ -6904,7 +6904,7 @@
       <c r="BM27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN27" s="5">
+      <c r="BN27" s="2">
         <v>2</v>
       </c>
       <c r="BO27" s="2" t="s">
@@ -7107,7 +7107,7 @@
       <c r="BM28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN28" s="6">
+      <c r="BN28" s="1">
         <v>2</v>
       </c>
       <c r="BO28" s="1" t="s">
@@ -7307,7 +7307,7 @@
       <c r="BM29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN29" s="6">
+      <c r="BN29" s="1">
         <v>1</v>
       </c>
       <c r="BO29" s="1" t="s">
@@ -7510,7 +7510,7 @@
       <c r="BM30" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN30" s="6">
+      <c r="BN30" s="1">
         <v>1</v>
       </c>
       <c r="BO30" s="1" t="s">
@@ -7713,7 +7713,7 @@
       <c r="BM31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="BN31" s="6">
+      <c r="BN31" s="1">
         <v>1</v>
       </c>
       <c r="BO31" s="1" t="s">

</xml_diff>